<commit_message>
Update on 10/29/18 with NFL Weeks 1-5 as training data and Week 6 as test data
</commit_message>
<xml_diff>
--- a/ner_eval.xlsx
+++ b/ner_eval.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="104">
   <si>
     <t>GAME RECAP ARTICLE</t>
   </si>
@@ -277,13 +277,64 @@
   </si>
   <si>
     <t>WEEK 5 (UNSEEN DATA)</t>
+  </si>
+  <si>
+    <t>WEEK 5 (SEEN DATA)</t>
+  </si>
+  <si>
+    <t>Δ</t>
+  </si>
+  <si>
+    <t>101118_eagles_giants</t>
+  </si>
+  <si>
+    <t>101418_bears_dolphins</t>
+  </si>
+  <si>
+    <t>101418_bills_texans</t>
+  </si>
+  <si>
+    <t>101418_buccaneers_falcons</t>
+  </si>
+  <si>
+    <t>101418_cardinals_vikings</t>
+  </si>
+  <si>
+    <t>101418_chargers_browns</t>
+  </si>
+  <si>
+    <t>101418_chiefs_patriots</t>
+  </si>
+  <si>
+    <t>101418-colts_jets</t>
+  </si>
+  <si>
+    <t>101418_jaguars_cowboys</t>
+  </si>
+  <si>
+    <t>101418_panthers_redskins</t>
+  </si>
+  <si>
+    <t>101418_rams_broncos</t>
+  </si>
+  <si>
+    <t>101418_ravens_titans</t>
+  </si>
+  <si>
+    <t>101418_seahawks_browns</t>
+  </si>
+  <si>
+    <t>101518_49ers_packers</t>
+  </si>
+  <si>
+    <t>WEEK 6 (UNSEEN DATA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +349,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -320,9 +378,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="F48" workbookViewId="0">
+      <selection activeCell="O74" sqref="O74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,17 +695,19 @@
     <col min="2" max="2" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" customWidth="1"/>
+    <col min="9" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" customWidth="1"/>
+    <col min="16" max="17" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,32 +720,32 @@
       <c r="D1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -698,34 +759,34 @@
         <f>B2/(B2+C2)</f>
         <v>0.82758620689655171</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>88</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7</v>
       </c>
-      <c r="I2">
-        <f>G2/(G2+H2)</f>
+      <c r="J2">
+        <f>H2/(H2+I2)</f>
         <v>0.9263157894736842</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>71</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>95</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>10</v>
       </c>
-      <c r="N2">
-        <f>L2/(L2+M2)</f>
+      <c r="P2">
+        <f>N2/(N2+O2)</f>
         <v>0.90476190476190477</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -739,34 +800,34 @@
         <f t="shared" ref="D3:D18" si="0">B3/(B3+C3)</f>
         <v>0.94623655913978499</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>74</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>5</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I18" si="1">G3/(G3+H3)</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J18" si="1">H3/(H3+I3)</f>
         <v>0.93670886075949367</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>72</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>102</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>11</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N17" si="2">L3/(L3+M3)</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P17" si="2">N3/(N3+O3)</f>
         <v>0.90265486725663713</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -780,34 +841,34 @@
         <f t="shared" si="0"/>
         <v>0.77551020408163263</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>72</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>9</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>73</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>68</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <f t="shared" si="2"/>
         <v>0.91891891891891897</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -821,34 +882,34 @@
         <f t="shared" si="0"/>
         <v>0.92783505154639179</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>85</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>20</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="1"/>
         <v>0.80952380952380953</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>74</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>87</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>9</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <f t="shared" si="2"/>
         <v>0.90625</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -862,34 +923,34 @@
         <f t="shared" si="0"/>
         <v>0.92307692307692313</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>81</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>12</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="1"/>
         <v>0.87096774193548387</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>75</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>90</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>9</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <f t="shared" si="2"/>
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -903,34 +964,34 @@
         <f t="shared" si="0"/>
         <v>0.86813186813186816</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>54</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>10</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="1"/>
         <v>0.84375</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>76</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>76</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>11</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <f t="shared" si="2"/>
         <v>0.87356321839080464</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -944,34 +1005,34 @@
         <f t="shared" si="0"/>
         <v>0.92156862745098034</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>24</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>116</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>17</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f t="shared" si="1"/>
         <v>0.8721804511278195</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>77</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>65</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>14</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <f t="shared" si="2"/>
         <v>0.82278481012658233</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -985,34 +1046,34 @@
         <f t="shared" si="0"/>
         <v>0.80808080808080807</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>82</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>10</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="1"/>
         <v>0.89130434782608692</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>78</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>74</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>14</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <f t="shared" si="2"/>
         <v>0.84090909090909094</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1026,34 +1087,34 @@
         <f t="shared" si="0"/>
         <v>0.84210526315789469</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>26</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>95</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>12</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="1"/>
         <v>0.88785046728971961</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>79</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>71</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>9</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <f t="shared" si="2"/>
         <v>0.88749999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1067,34 +1128,34 @@
         <f t="shared" si="0"/>
         <v>0.91304347826086951</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>27</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>84</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>6</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f t="shared" si="1"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>80</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>70</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>14</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1108,34 +1169,34 @@
         <f t="shared" si="0"/>
         <v>0.79487179487179482</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>28</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>84</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>16</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="1"/>
         <v>0.84</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>81</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>94</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>15</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <f t="shared" si="2"/>
         <v>0.86238532110091748</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1149,34 +1210,34 @@
         <f t="shared" si="0"/>
         <v>0.8651685393258427</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>29</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>86</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>9</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f t="shared" si="1"/>
         <v>0.90526315789473688</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>82</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>75</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>15</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1190,34 +1251,34 @@
         <f t="shared" si="0"/>
         <v>0.9363636363636364</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>30</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>72</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>19</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f t="shared" si="1"/>
         <v>0.79120879120879117</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>83</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>91</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>20</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <f t="shared" si="2"/>
         <v>0.81981981981981977</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1231,34 +1292,34 @@
         <f t="shared" si="0"/>
         <v>0.8666666666666667</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>31</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>83</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>16</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="1"/>
         <v>0.83838383838383834</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>84</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>91</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>14</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <f t="shared" si="2"/>
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1272,34 +1333,34 @@
         <f t="shared" si="0"/>
         <v>0.87</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>32</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>65</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>14</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="1"/>
         <v>0.82278481012658233</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>85</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>79</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>16</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <f t="shared" si="2"/>
         <v>0.83157894736842108</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1313,36 +1374,36 @@
         <f t="shared" si="0"/>
         <v>0.82828282828282829</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>33</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>79</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>14</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="1"/>
         <v>0.84946236559139787</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>86</v>
       </c>
-      <c r="L17">
-        <f>SUM(L2:L16)</f>
+      <c r="N17">
+        <f>SUM(N2:N16)</f>
         <v>1228</v>
       </c>
-      <c r="M17">
-        <f>SUM(M2:M16)</f>
+      <c r="O17">
+        <f>SUM(O2:O16)</f>
         <v>187</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <f t="shared" si="2"/>
         <v>0.86784452296819792</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1358,23 +1419,23 @@
         <f t="shared" si="0"/>
         <v>0.87051792828685259</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>34</v>
-      </c>
-      <c r="G18">
-        <f>SUM(G2:G17)</f>
-        <v>1300</v>
       </c>
       <c r="H18">
         <f>SUM(H2:H17)</f>
+        <v>1300</v>
+      </c>
+      <c r="I18">
+        <f>SUM(I2:I17)</f>
         <v>196</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="1"/>
         <v>0.86898395721925137</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,20 +1448,20 @@
       <c r="D20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1414,21 +1475,21 @@
         <f>B21/(B21+C21)</f>
         <v>0.8257575757575758</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>54</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>77</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>18</v>
       </c>
-      <c r="I21">
-        <f>G21/(G21+H21)</f>
+      <c r="J21">
+        <f>H21/(H21+I21)</f>
         <v>0.81052631578947365</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1442,21 +1503,21 @@
         <f t="shared" ref="D22:D37" si="3">B22/(B22+C22)</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>55</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>73</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>7</v>
       </c>
-      <c r="I22">
-        <f t="shared" ref="I22:I35" si="4">G22/(G22+H22)</f>
+      <c r="J22">
+        <f t="shared" ref="J22:J31" si="4">H22/(H22+I22)</f>
         <v>0.91249999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1470,21 +1531,21 @@
         <f t="shared" si="3"/>
         <v>0.8910891089108911</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>56</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>85</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>19</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f t="shared" si="4"/>
         <v>0.81730769230769229</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1498,21 +1559,21 @@
         <f t="shared" si="3"/>
         <v>0.8045977011494253</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>57</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>66</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>12</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f t="shared" si="4"/>
         <v>0.84615384615384615</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1526,21 +1587,21 @@
         <f t="shared" si="3"/>
         <v>0.80208333333333337</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>58</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>72</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>10</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f t="shared" si="4"/>
         <v>0.87804878048780488</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1554,21 +1615,21 @@
         <f t="shared" si="3"/>
         <v>0.83</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>59</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>81</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>14</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f t="shared" si="4"/>
         <v>0.85263157894736841</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1582,21 +1643,21 @@
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>60</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>103</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>10</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f t="shared" si="4"/>
         <v>0.91150442477876104</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1610,21 +1671,21 @@
         <f t="shared" si="3"/>
         <v>0.8392857142857143</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>61</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>79</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>12</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f t="shared" si="4"/>
         <v>0.86813186813186816</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1638,21 +1699,21 @@
         <f t="shared" si="3"/>
         <v>0.92105263157894735</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>62</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>75</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>5</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <f t="shared" si="4"/>
         <v>0.9375</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1666,21 +1727,21 @@
         <f t="shared" si="3"/>
         <v>0.92405063291139244</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>63</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>85</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>6</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <f t="shared" si="4"/>
         <v>0.93406593406593408</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1694,21 +1755,21 @@
         <f t="shared" si="3"/>
         <v>0.82608695652173914</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>64</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>99</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>14</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <f t="shared" si="4"/>
         <v>0.87610619469026552</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1722,21 +1783,21 @@
         <f t="shared" si="3"/>
         <v>0.81395348837209303</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>70</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>74</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>2</v>
       </c>
-      <c r="I32">
-        <f>G32/(G32+H32)</f>
+      <c r="J32">
+        <f>H32/(H32+I32)</f>
         <v>0.97368421052631582</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1750,21 +1811,21 @@
         <f t="shared" si="3"/>
         <v>0.85567010309278346</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>65</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>78</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>6</v>
       </c>
-      <c r="I33">
-        <f>G33/(G33+H33)</f>
+      <c r="J33">
+        <f>H33/(H33+I33)</f>
         <v>0.9285714285714286</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1778,21 +1839,21 @@
         <f t="shared" si="3"/>
         <v>0.90196078431372551</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>66</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>65</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>14</v>
       </c>
-      <c r="I34">
-        <f>G34/(G34+H34)</f>
+      <c r="J34">
+        <f>H34/(H34+I34)</f>
         <v>0.82278481012658233</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -1806,21 +1867,21 @@
         <f t="shared" si="3"/>
         <v>0.86486486486486491</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>67</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>70</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>12</v>
       </c>
-      <c r="I35">
-        <f>G35/(G35+H35)</f>
+      <c r="J35">
+        <f>H35/(H35+I35)</f>
         <v>0.85365853658536583</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1834,23 +1895,23 @@
         <f t="shared" si="3"/>
         <v>0.79629629629629628</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>68</v>
-      </c>
-      <c r="G36">
-        <f>SUM(G21:G35)</f>
-        <v>1182</v>
       </c>
       <c r="H36">
         <f>SUM(H21:H35)</f>
+        <v>1182</v>
+      </c>
+      <c r="I36">
+        <f>SUM(I21:I35)</f>
         <v>161</v>
       </c>
-      <c r="I36">
-        <f>G36/(G36+H36)</f>
+      <c r="J36">
+        <f>H36/(H36+I36)</f>
         <v>0.88011913626209981</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1865,6 +1926,1784 @@
       <c r="D37">
         <f t="shared" si="3"/>
         <v>0.84825396825396826</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>99</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <f>B41/(B41+C41)</f>
+        <v>0.86086956521739133</v>
+      </c>
+      <c r="E41">
+        <f>D41-D2</f>
+        <v>3.3283358320839618E-2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41">
+        <v>88</v>
+      </c>
+      <c r="I41">
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <f>H41/(H41+I41)</f>
+        <v>0.93617021276595747</v>
+      </c>
+      <c r="K41">
+        <f>J41-J2</f>
+        <v>9.8544232922732622E-3</v>
+      </c>
+      <c r="M41" t="s">
+        <v>71</v>
+      </c>
+      <c r="N41">
+        <v>93</v>
+      </c>
+      <c r="O41">
+        <v>7</v>
+      </c>
+      <c r="P41">
+        <f>N41/(N41+O41)</f>
+        <v>0.93</v>
+      </c>
+      <c r="Q41">
+        <f>P41-P2</f>
+        <v>2.5238095238095282E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42">
+        <v>87</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42:D57" si="5">B42/(B42+C42)</f>
+        <v>0.93548387096774188</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42:E57" si="6">D42-D3</f>
+        <v>-1.0752688172043112E-2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42">
+        <v>77</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <f t="shared" ref="J42:J57" si="7">H42/(H42+I42)</f>
+        <v>0.98717948717948723</v>
+      </c>
+      <c r="K42">
+        <f t="shared" ref="K42:K57" si="8">J42-J3</f>
+        <v>5.0470626419993558E-2</v>
+      </c>
+      <c r="M42" t="s">
+        <v>72</v>
+      </c>
+      <c r="N42">
+        <v>101</v>
+      </c>
+      <c r="O42">
+        <v>13</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ref="P42:P56" si="9">N42/(N42+O42)</f>
+        <v>0.88596491228070173</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" ref="Q42:Q56" si="10">P42-P3</f>
+        <v>-1.6689954975935395E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>83</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="5"/>
+        <v>0.92222222222222228</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="6"/>
+        <v>0.14671201814058965</v>
+      </c>
+      <c r="G43" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43">
+        <v>69</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="7"/>
+        <v>0.87341772151898733</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="8"/>
+        <v>-1.5471167369901506E-2</v>
+      </c>
+      <c r="M43" t="s">
+        <v>73</v>
+      </c>
+      <c r="N43">
+        <v>73</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="9"/>
+        <v>0.98648648648648651</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="10"/>
+        <v>6.7567567567567544E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>89</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="5"/>
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="6"/>
+        <v>-7.5171821305841657E-4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44">
+        <v>84</v>
+      </c>
+      <c r="I44">
+        <v>19</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="7"/>
+        <v>0.81553398058252424</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="8"/>
+        <v>6.0101710587147084E-3</v>
+      </c>
+      <c r="M44" t="s">
+        <v>74</v>
+      </c>
+      <c r="N44">
+        <v>87</v>
+      </c>
+      <c r="O44">
+        <v>10</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="9"/>
+        <v>0.89690721649484539</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="10"/>
+        <v>-9.342783505154606E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45">
+        <v>83</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="5"/>
+        <v>0.94318181818181823</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="6"/>
+        <v>2.0104895104895104E-2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45">
+        <v>77</v>
+      </c>
+      <c r="I45">
+        <v>13</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="7"/>
+        <v>0.85555555555555551</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="8"/>
+        <v>-1.5412186379928361E-2</v>
+      </c>
+      <c r="M45" t="s">
+        <v>75</v>
+      </c>
+      <c r="N45">
+        <v>92</v>
+      </c>
+      <c r="O45">
+        <v>3</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="9"/>
+        <v>0.96842105263157896</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="10"/>
+        <v>5.93301435406699E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>86</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="5"/>
+        <v>0.97727272727272729</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="6"/>
+        <v>0.10914085914085914</v>
+      </c>
+      <c r="G46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46">
+        <v>55</v>
+      </c>
+      <c r="I46">
+        <v>7</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="7"/>
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="8"/>
+        <v>4.3346774193548376E-2</v>
+      </c>
+      <c r="M46" t="s">
+        <v>76</v>
+      </c>
+      <c r="N46">
+        <v>77</v>
+      </c>
+      <c r="O46">
+        <v>11</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="9"/>
+        <v>0.875</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="10"/>
+        <v>1.4367816091953589E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>95</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="5"/>
+        <v>0.92233009708737868</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="6"/>
+        <v>7.6146963639833753E-4</v>
+      </c>
+      <c r="G47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47">
+        <v>117</v>
+      </c>
+      <c r="I47">
+        <v>8</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="7"/>
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="8"/>
+        <v>6.3819548872180554E-2</v>
+      </c>
+      <c r="M47" t="s">
+        <v>77</v>
+      </c>
+      <c r="N47">
+        <v>74</v>
+      </c>
+      <c r="O47">
+        <v>3</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="9"/>
+        <v>0.96103896103896103</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="10"/>
+        <v>0.13825415091237869</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>84</v>
+      </c>
+      <c r="C48">
+        <v>12</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="5"/>
+        <v>0.875</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>6.6919191919191934E-2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48">
+        <v>84</v>
+      </c>
+      <c r="I48">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="7"/>
+        <v>0.90322580645161288</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="8"/>
+        <v>1.192145862552596E-2</v>
+      </c>
+      <c r="M48" t="s">
+        <v>78</v>
+      </c>
+      <c r="N48">
+        <v>77</v>
+      </c>
+      <c r="O48">
+        <v>7</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="9"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="10"/>
+        <v>7.575757575757569E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>65</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="5"/>
+        <v>0.8904109589041096</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="6"/>
+        <v>4.8305695746214905E-2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>26</v>
+      </c>
+      <c r="H49">
+        <v>93</v>
+      </c>
+      <c r="I49">
+        <v>12</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="7"/>
+        <v>0.88571428571428568</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="8"/>
+        <v>-2.1361815754339375E-3</v>
+      </c>
+      <c r="M49" t="s">
+        <v>79</v>
+      </c>
+      <c r="N49">
+        <v>74</v>
+      </c>
+      <c r="O49">
+        <v>6</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="9"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="10"/>
+        <v>3.7500000000000089E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>79</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="5"/>
+        <v>0.90804597701149425</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="6"/>
+        <v>-4.997501249375258E-3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>27</v>
+      </c>
+      <c r="H50">
+        <v>81</v>
+      </c>
+      <c r="I50">
+        <v>10</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="7"/>
+        <v>0.89010989010989006</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="8"/>
+        <v>-4.3223443223443292E-2</v>
+      </c>
+      <c r="M50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N50">
+        <v>72</v>
+      </c>
+      <c r="O50">
+        <v>6</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="9"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="10"/>
+        <v>8.9743589743589758E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51">
+        <v>66</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="5"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="6"/>
+        <v>0.12179487179487181</v>
+      </c>
+      <c r="G51" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51">
+        <v>75</v>
+      </c>
+      <c r="I51">
+        <v>14</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="7"/>
+        <v>0.84269662921348309</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="8"/>
+        <v>2.696629213483126E-3</v>
+      </c>
+      <c r="M51" t="s">
+        <v>81</v>
+      </c>
+      <c r="N51">
+        <v>99</v>
+      </c>
+      <c r="O51">
+        <v>6</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="9"/>
+        <v>0.94285714285714284</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="10"/>
+        <v>8.0471821756225359E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52">
+        <v>80</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="5"/>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="6"/>
+        <v>7.6007931262392581E-2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52">
+        <v>88</v>
+      </c>
+      <c r="I52">
+        <v>11</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="7"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="8"/>
+        <v>-1.6374269005848041E-2</v>
+      </c>
+      <c r="M52" t="s">
+        <v>82</v>
+      </c>
+      <c r="N52">
+        <v>83</v>
+      </c>
+      <c r="O52">
+        <v>7</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="9"/>
+        <v>0.92222222222222228</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="10"/>
+        <v>8.8888888888888906E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53">
+        <v>101</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="5"/>
+        <v>0.92660550458715596</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="6"/>
+        <v>-9.7581317764804387E-3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53">
+        <v>77</v>
+      </c>
+      <c r="I53">
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="7"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="8"/>
+        <v>5.4945054945054972E-2</v>
+      </c>
+      <c r="M53" t="s">
+        <v>83</v>
+      </c>
+      <c r="N53">
+        <v>92</v>
+      </c>
+      <c r="O53">
+        <v>13</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="9"/>
+        <v>0.87619047619047619</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="10"/>
+        <v>5.6370656370656413E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54">
+        <v>66</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="5"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="6"/>
+        <v>4.9999999999999933E-2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54">
+        <v>86</v>
+      </c>
+      <c r="I54">
+        <v>14</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="7"/>
+        <v>0.86</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="8"/>
+        <v>2.1616161616161644E-2</v>
+      </c>
+      <c r="M54" t="s">
+        <v>84</v>
+      </c>
+      <c r="N54">
+        <v>96</v>
+      </c>
+      <c r="O54">
+        <v>4</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="9"/>
+        <v>0.96</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="10"/>
+        <v>9.3333333333333268E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>83</v>
+      </c>
+      <c r="C55">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="5"/>
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="6"/>
+        <v>-5.4166666666666252E-3</v>
+      </c>
+      <c r="G55" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55">
+        <v>69</v>
+      </c>
+      <c r="I55">
+        <v>7</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="7"/>
+        <v>0.90789473684210531</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="8"/>
+        <v>8.5109926715522977E-2</v>
+      </c>
+      <c r="M55" t="s">
+        <v>85</v>
+      </c>
+      <c r="N55">
+        <v>85</v>
+      </c>
+      <c r="O55">
+        <v>10</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="9"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="10"/>
+        <v>6.315789473684208E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56">
+        <v>85</v>
+      </c>
+      <c r="C56">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="5"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="6"/>
+        <v>6.6454013822434876E-2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>33</v>
+      </c>
+      <c r="H56">
+        <v>77</v>
+      </c>
+      <c r="I56">
+        <v>12</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="7"/>
+        <v>0.8651685393258427</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="8"/>
+        <v>1.5706173734444828E-2</v>
+      </c>
+      <c r="M56" t="s">
+        <v>87</v>
+      </c>
+      <c r="N56">
+        <f>SUM(N41:N55)</f>
+        <v>1275</v>
+      </c>
+      <c r="O56">
+        <f>SUM(O41:O55)</f>
+        <v>107</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="9"/>
+        <v>0.92257597684515191</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="10"/>
+        <v>5.4731453876953995E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57">
+        <f>SUM(B41:B56)</f>
+        <v>1331</v>
+      </c>
+      <c r="C57">
+        <f>SUM(C41:C56)</f>
+        <v>127</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="5"/>
+        <v>0.91289437585733879</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="6"/>
+        <v>4.2376447570486198E-2</v>
+      </c>
+      <c r="G57" t="s">
+        <v>34</v>
+      </c>
+      <c r="H57">
+        <f>SUM(H41:H56)</f>
+        <v>1297</v>
+      </c>
+      <c r="I57">
+        <f>SUM(I41:I56)</f>
+        <v>167</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="7"/>
+        <v>0.88592896174863389</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="8"/>
+        <v>1.6945004529382524E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q59" s="2"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60">
+        <v>110</v>
+      </c>
+      <c r="C60">
+        <v>19</v>
+      </c>
+      <c r="D60">
+        <f>B60/(B60+C60)</f>
+        <v>0.8527131782945736</v>
+      </c>
+      <c r="E60">
+        <f>D60-D21</f>
+        <v>2.6955602536997803E-2</v>
+      </c>
+      <c r="G60" t="s">
+        <v>54</v>
+      </c>
+      <c r="H60">
+        <v>85</v>
+      </c>
+      <c r="I60">
+        <v>12</v>
+      </c>
+      <c r="J60">
+        <f>H60/(H60+I60)</f>
+        <v>0.87628865979381443</v>
+      </c>
+      <c r="K60">
+        <f>J60-J21</f>
+        <v>6.5762344004340778E-2</v>
+      </c>
+      <c r="M60" t="s">
+        <v>89</v>
+      </c>
+      <c r="N60">
+        <v>88</v>
+      </c>
+      <c r="O60">
+        <v>13</v>
+      </c>
+      <c r="P60">
+        <f>N60/(N60+O60)</f>
+        <v>0.87128712871287128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61">
+        <v>86</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ref="D61:D76" si="11">B61/(B61+C61)</f>
+        <v>0.94505494505494503</v>
+      </c>
+      <c r="E61">
+        <f t="shared" ref="E61:E76" si="12">D61-D22</f>
+        <v>5.6166056166056189E-2</v>
+      </c>
+      <c r="G61" t="s">
+        <v>55</v>
+      </c>
+      <c r="H61">
+        <v>73</v>
+      </c>
+      <c r="I61">
+        <v>7</v>
+      </c>
+      <c r="J61">
+        <f t="shared" ref="J61:J70" si="13">H61/(H61+I61)</f>
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="K61">
+        <f t="shared" ref="K61:K75" si="14">J61-J22</f>
+        <v>0</v>
+      </c>
+      <c r="M61" t="s">
+        <v>90</v>
+      </c>
+      <c r="N61">
+        <v>75</v>
+      </c>
+      <c r="O61">
+        <v>7</v>
+      </c>
+      <c r="P61">
+        <f t="shared" ref="P61:P74" si="15">N61/(N61+O61)</f>
+        <v>0.91463414634146345</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62">
+        <v>96</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="11"/>
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="12"/>
+        <v>7.860786078607862E-2</v>
+      </c>
+      <c r="G62" t="s">
+        <v>56</v>
+      </c>
+      <c r="H62">
+        <v>89</v>
+      </c>
+      <c r="I62">
+        <v>12</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="13"/>
+        <v>0.88118811881188119</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="14"/>
+        <v>6.3880426504188903E-2</v>
+      </c>
+      <c r="M62" t="s">
+        <v>91</v>
+      </c>
+      <c r="N62">
+        <v>76</v>
+      </c>
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="15"/>
+        <v>0.98701298701298701</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63">
+        <v>73</v>
+      </c>
+      <c r="C63">
+        <v>12</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="11"/>
+        <v>0.85882352941176465</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="12"/>
+        <v>5.4225828262339348E-2</v>
+      </c>
+      <c r="G63" t="s">
+        <v>57</v>
+      </c>
+      <c r="H63">
+        <v>66</v>
+      </c>
+      <c r="I63">
+        <v>10</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="13"/>
+        <v>0.86842105263157898</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="14"/>
+        <v>2.2267206477732837E-2</v>
+      </c>
+      <c r="M63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N63">
+        <v>83</v>
+      </c>
+      <c r="O63">
+        <v>9</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="15"/>
+        <v>0.90217391304347827</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64">
+        <v>77</v>
+      </c>
+      <c r="C64">
+        <v>18</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="11"/>
+        <v>0.81052631578947365</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="12"/>
+        <v>8.44298245614028E-3</v>
+      </c>
+      <c r="G64" t="s">
+        <v>58</v>
+      </c>
+      <c r="H64">
+        <v>75</v>
+      </c>
+      <c r="I64">
+        <v>6</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="13"/>
+        <v>0.92592592592592593</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="14"/>
+        <v>4.7877145438121049E-2</v>
+      </c>
+      <c r="M64" t="s">
+        <v>93</v>
+      </c>
+      <c r="N64">
+        <v>85</v>
+      </c>
+      <c r="O64">
+        <v>8</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="15"/>
+        <v>0.91397849462365588</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65">
+        <v>89</v>
+      </c>
+      <c r="C65">
+        <v>11</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="11"/>
+        <v>0.89</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="12"/>
+        <v>6.0000000000000053E-2</v>
+      </c>
+      <c r="G65" t="s">
+        <v>59</v>
+      </c>
+      <c r="H65">
+        <v>84</v>
+      </c>
+      <c r="I65">
+        <v>6</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="13"/>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="14"/>
+        <v>8.0701754385964941E-2</v>
+      </c>
+      <c r="M65" t="s">
+        <v>94</v>
+      </c>
+      <c r="N65">
+        <v>86</v>
+      </c>
+      <c r="O65">
+        <v>12</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="15"/>
+        <v>0.87755102040816324</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66">
+        <v>87</v>
+      </c>
+      <c r="C66">
+        <v>16</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="11"/>
+        <v>0.84466019417475724</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="12"/>
+        <v>4.4660194174757195E-2</v>
+      </c>
+      <c r="G66" t="s">
+        <v>60</v>
+      </c>
+      <c r="H66">
+        <v>104</v>
+      </c>
+      <c r="I66">
+        <v>5</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="13"/>
+        <v>0.95412844036697253</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="14"/>
+        <v>4.2624015588211495E-2</v>
+      </c>
+      <c r="M66" t="s">
+        <v>95</v>
+      </c>
+      <c r="N66">
+        <v>83</v>
+      </c>
+      <c r="O66">
+        <v>9</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="15"/>
+        <v>0.90217391304347827</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67">
+        <v>99</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="11"/>
+        <v>0.93396226415094341</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="12"/>
+        <v>9.4676549865229109E-2</v>
+      </c>
+      <c r="G67" t="s">
+        <v>61</v>
+      </c>
+      <c r="H67">
+        <v>78</v>
+      </c>
+      <c r="I67">
+        <v>8</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="13"/>
+        <v>0.90697674418604646</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="14"/>
+        <v>3.8844876054178301E-2</v>
+      </c>
+      <c r="M67" t="s">
+        <v>96</v>
+      </c>
+      <c r="N67">
+        <v>114</v>
+      </c>
+      <c r="O67">
+        <v>13</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="15"/>
+        <v>0.89763779527559051</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68">
+        <v>102</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="11"/>
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="12"/>
+        <v>2.3391812865497075E-2</v>
+      </c>
+      <c r="G68" t="s">
+        <v>62</v>
+      </c>
+      <c r="H68">
+        <v>70</v>
+      </c>
+      <c r="I68">
+        <v>9</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="13"/>
+        <v>0.88607594936708856</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="14"/>
+        <v>-5.1424050632911444E-2</v>
+      </c>
+      <c r="M68" t="s">
+        <v>97</v>
+      </c>
+      <c r="N68">
+        <v>71</v>
+      </c>
+      <c r="O68">
+        <v>11</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="15"/>
+        <v>0.86585365853658536</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69">
+        <v>76</v>
+      </c>
+      <c r="C69">
+        <v>9</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="11"/>
+        <v>0.89411764705882357</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="12"/>
+        <v>-2.9932985852568872E-2</v>
+      </c>
+      <c r="G69" t="s">
+        <v>63</v>
+      </c>
+      <c r="H69">
+        <v>83</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="13"/>
+        <v>0.94318181818181823</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="14"/>
+        <v>9.1158841158841541E-3</v>
+      </c>
+      <c r="M69" t="s">
+        <v>98</v>
+      </c>
+      <c r="N69">
+        <v>77</v>
+      </c>
+      <c r="O69">
+        <v>9</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="15"/>
+        <v>0.89534883720930236</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>47</v>
+      </c>
+      <c r="B70">
+        <v>78</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="11"/>
+        <v>0.90697674418604646</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="12"/>
+        <v>8.0889787664307322E-2</v>
+      </c>
+      <c r="G70" t="s">
+        <v>64</v>
+      </c>
+      <c r="H70">
+        <v>104</v>
+      </c>
+      <c r="I70">
+        <v>6</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="13"/>
+        <v>0.94545454545454544</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="14"/>
+        <v>6.934835076427992E-2</v>
+      </c>
+      <c r="M70" t="s">
+        <v>99</v>
+      </c>
+      <c r="N70">
+        <v>87</v>
+      </c>
+      <c r="O70">
+        <v>15</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="15"/>
+        <v>0.8529411764705882</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71">
+        <v>74</v>
+      </c>
+      <c r="C71">
+        <v>13</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="11"/>
+        <v>0.85057471264367812</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="12"/>
+        <v>3.6621224271585096E-2</v>
+      </c>
+      <c r="G71" t="s">
+        <v>70</v>
+      </c>
+      <c r="H71">
+        <v>71</v>
+      </c>
+      <c r="I71">
+        <v>3</v>
+      </c>
+      <c r="J71">
+        <f>H71/(H71+I71)</f>
+        <v>0.95945945945945943</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="14"/>
+        <v>-1.4224751066856389E-2</v>
+      </c>
+      <c r="M71" t="s">
+        <v>100</v>
+      </c>
+      <c r="N71">
+        <v>83</v>
+      </c>
+      <c r="O71">
+        <v>12</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="15"/>
+        <v>0.87368421052631584</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72">
+        <v>82</v>
+      </c>
+      <c r="C72">
+        <v>9</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="11"/>
+        <v>0.90109890109890112</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="12"/>
+        <v>4.5428798006117654E-2</v>
+      </c>
+      <c r="G72" t="s">
+        <v>65</v>
+      </c>
+      <c r="H72">
+        <v>77</v>
+      </c>
+      <c r="I72">
+        <v>6</v>
+      </c>
+      <c r="J72">
+        <f>H72/(H72+I72)</f>
+        <v>0.92771084337349397</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="14"/>
+        <v>-8.6058519793463795E-4</v>
+      </c>
+      <c r="M72" t="s">
+        <v>101</v>
+      </c>
+      <c r="N72">
+        <v>70</v>
+      </c>
+      <c r="O72">
+        <v>19</v>
+      </c>
+      <c r="P72">
+        <f t="shared" si="15"/>
+        <v>0.7865168539325843</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73">
+        <v>92</v>
+      </c>
+      <c r="C73">
+        <v>8</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="11"/>
+        <v>0.92</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="12"/>
+        <v>1.8039215686274535E-2</v>
+      </c>
+      <c r="G73" t="s">
+        <v>66</v>
+      </c>
+      <c r="H73">
+        <v>67</v>
+      </c>
+      <c r="I73">
+        <v>7</v>
+      </c>
+      <c r="J73">
+        <f>H73/(H73+I73)</f>
+        <v>0.90540540540540537</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="14"/>
+        <v>8.2620595278823039E-2</v>
+      </c>
+      <c r="M73" t="s">
+        <v>102</v>
+      </c>
+      <c r="N73">
+        <v>87</v>
+      </c>
+      <c r="O73">
+        <v>14</v>
+      </c>
+      <c r="P73">
+        <f t="shared" si="15"/>
+        <v>0.86138613861386137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74">
+        <v>67</v>
+      </c>
+      <c r="C74">
+        <v>7</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="11"/>
+        <v>0.90540540540540537</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="12"/>
+        <v>4.054054054054046E-2</v>
+      </c>
+      <c r="G74" t="s">
+        <v>67</v>
+      </c>
+      <c r="H74">
+        <v>70</v>
+      </c>
+      <c r="I74">
+        <v>14</v>
+      </c>
+      <c r="J74">
+        <f>H74/(H74+I74)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="14"/>
+        <v>-2.0325203252032464E-2</v>
+      </c>
+      <c r="M74" t="s">
+        <v>103</v>
+      </c>
+      <c r="N74">
+        <f>SUM(N60:N73)</f>
+        <v>1165</v>
+      </c>
+      <c r="O74">
+        <f>SUM(O60:O73)</f>
+        <v>152</v>
+      </c>
+      <c r="P74">
+        <f t="shared" si="15"/>
+        <v>0.8845861807137434</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75">
+        <v>91</v>
+      </c>
+      <c r="C75">
+        <v>16</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="11"/>
+        <v>0.85046728971962615</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="12"/>
+        <v>5.4170993423329872E-2</v>
+      </c>
+      <c r="G75" t="s">
+        <v>68</v>
+      </c>
+      <c r="H75">
+        <f>SUM(H60:H74)</f>
+        <v>1196</v>
+      </c>
+      <c r="I75">
+        <f>SUM(I60:I74)</f>
+        <v>116</v>
+      </c>
+      <c r="J75">
+        <f>H75/(H75+I75)</f>
+        <v>0.91158536585365857</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="14"/>
+        <v>3.1466229591558759E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76">
+        <f>SUM(B60:B75)</f>
+        <v>1379</v>
+      </c>
+      <c r="C76">
+        <f>SUM(C60:C75)</f>
+        <v>167</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="11"/>
+        <v>0.89197930142302717</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="12"/>
+        <v>4.3725333169058911E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full updates for Week 6 as unseen data set
</commit_message>
<xml_diff>
--- a/ner_eval.xlsx
+++ b/ner_eval.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="105">
   <si>
     <t>GAME RECAP ARTICLE</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>WEEK 6 (UNSEEN DATA)</t>
+  </si>
+  <si>
+    <t>101418_steelers_browns</t>
   </si>
 </sst>
 </file>
@@ -3004,7 +3007,7 @@
         <v>7</v>
       </c>
       <c r="P61">
-        <f t="shared" ref="P61:P74" si="15">N61/(N61+O61)</f>
+        <f t="shared" ref="P61:P75" si="15">N61/(N61+O61)</f>
         <v>0.91463414634146345</v>
       </c>
     </row>
@@ -3583,7 +3586,7 @@
         <v>8.2620595278823039E-2</v>
       </c>
       <c r="M73" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="N73">
         <v>87</v>
@@ -3632,19 +3635,17 @@
         <v>-2.0325203252032464E-2</v>
       </c>
       <c r="M74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N74">
-        <f>SUM(N60:N73)</f>
-        <v>1165</v>
+        <v>73</v>
       </c>
       <c r="O74">
-        <f>SUM(O60:O73)</f>
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="P74">
         <f t="shared" si="15"/>
-        <v>0.8845861807137434</v>
+        <v>0.87951807228915657</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -3683,6 +3684,21 @@
       <c r="K75">
         <f t="shared" si="14"/>
         <v>3.1466229591558759E-2</v>
+      </c>
+      <c r="M75" t="s">
+        <v>103</v>
+      </c>
+      <c r="N75">
+        <f>SUM(N60:N74)</f>
+        <v>1238</v>
+      </c>
+      <c r="O75">
+        <f>SUM(O60:O74)</f>
+        <v>162</v>
+      </c>
+      <c r="P75">
+        <f t="shared" si="15"/>
+        <v>0.88428571428571423</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
pushing updates for Weeks 1-6 as SEEN and Week 7 as UNSEEN
</commit_message>
<xml_diff>
--- a/ner_eval.xlsx
+++ b/ner_eval.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="121">
   <si>
     <t>GAME RECAP ARTICLE</t>
   </si>
@@ -321,16 +321,64 @@
     <t>101418_ravens_titans</t>
   </si>
   <si>
-    <t>101418_seahawks_browns</t>
-  </si>
-  <si>
     <t>101518_49ers_packers</t>
   </si>
   <si>
     <t>WEEK 6 (UNSEEN DATA)</t>
   </si>
   <si>
-    <t>101418_steelers_browns</t>
+    <t>101418_steelers_bengals</t>
+  </si>
+  <si>
+    <t>101418_seahawks_raiders</t>
+  </si>
+  <si>
+    <t>WEEK 6 (SEEN DATA)</t>
+  </si>
+  <si>
+    <t>101818_broncos_cardinals</t>
+  </si>
+  <si>
+    <t>102118_bengals_chiefs</t>
+  </si>
+  <si>
+    <t>102118_bills_colts</t>
+  </si>
+  <si>
+    <t>102118_browns_buccaneers</t>
+  </si>
+  <si>
+    <t>102118_cowboys_redskins</t>
+  </si>
+  <si>
+    <t>102118_lions_dolphins</t>
+  </si>
+  <si>
+    <t>102118_panthers_eagles</t>
+  </si>
+  <si>
+    <t>102118_patriots_bears</t>
+  </si>
+  <si>
+    <t>102118_rams_49ers</t>
+  </si>
+  <si>
+    <t>102118_saints_ravens</t>
+  </si>
+  <si>
+    <t>102118_texans_jaguars</t>
+  </si>
+  <si>
+    <t>102118_titans_chargers</t>
+  </si>
+  <si>
+    <t>102118_vikings_jets</t>
+  </si>
+  <si>
+    <t>102218_giants_falcons</t>
+  </si>
+  <si>
+    <t>WEEK 7 (UNSEEN DATA)</t>
   </si>
 </sst>
 </file>
@@ -686,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:V115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F48" workbookViewId="0">
-      <selection activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" topLeftCell="K86" workbookViewId="0">
+      <selection activeCell="T93" sqref="T93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,6 +756,8 @@
     <col min="14" max="14" width="7.28515625" customWidth="1"/>
     <col min="15" max="15" width="7.5703125" customWidth="1"/>
     <col min="16" max="17" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="25.85546875" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3158,7 +3208,7 @@
         <v>0.91397849462365588</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -3207,7 +3257,7 @@
         <v>0.87755102040816324</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -3256,7 +3306,7 @@
         <v>0.90217391304347827</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -3305,7 +3355,7 @@
         <v>0.89763779527559051</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>45</v>
       </c>
@@ -3354,7 +3404,7 @@
         <v>0.86585365853658536</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>46</v>
       </c>
@@ -3403,7 +3453,7 @@
         <v>0.89534883720930236</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -3452,7 +3502,7 @@
         <v>0.8529411764705882</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -3501,7 +3551,7 @@
         <v>0.87368421052631584</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>49</v>
       </c>
@@ -3537,7 +3587,7 @@
         <v>-8.6058519793463795E-4</v>
       </c>
       <c r="M72" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N72">
         <v>70</v>
@@ -3550,7 +3600,7 @@
         <v>0.7865168539325843</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>50</v>
       </c>
@@ -3586,7 +3636,7 @@
         <v>8.2620595278823039E-2</v>
       </c>
       <c r="M73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N73">
         <v>87</v>
@@ -3599,7 +3649,7 @@
         <v>0.86138613861386137</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>51</v>
       </c>
@@ -3635,7 +3685,7 @@
         <v>-2.0325203252032464E-2</v>
       </c>
       <c r="M74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N74">
         <v>73</v>
@@ -3648,7 +3698,7 @@
         <v>0.87951807228915657</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -3686,7 +3736,7 @@
         <v>3.1466229591558759E-2</v>
       </c>
       <c r="M75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N75">
         <f>SUM(N60:N74)</f>
@@ -3701,7 +3751,7 @@
         <v>0.88428571428571423</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -3720,6 +3770,2072 @@
       <c r="E76">
         <f t="shared" si="12"/>
         <v>4.3725333169058911E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q79" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="S79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T79" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V79" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80">
+        <v>108</v>
+      </c>
+      <c r="C80">
+        <v>5</v>
+      </c>
+      <c r="D80">
+        <f>B80/(B80+C80)</f>
+        <v>0.95575221238938057</v>
+      </c>
+      <c r="E80">
+        <f>D80-D41</f>
+        <v>9.4882647171989243E-2</v>
+      </c>
+      <c r="G80" t="s">
+        <v>18</v>
+      </c>
+      <c r="H80">
+        <v>90</v>
+      </c>
+      <c r="I80">
+        <v>6</v>
+      </c>
+      <c r="J80">
+        <f>H80/(H80+I80)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="K80">
+        <f>J80-J41</f>
+        <v>1.3297872340425343E-3</v>
+      </c>
+      <c r="M80" t="s">
+        <v>71</v>
+      </c>
+      <c r="N80">
+        <v>100</v>
+      </c>
+      <c r="O80">
+        <v>2</v>
+      </c>
+      <c r="P80">
+        <f>N80/(N80+O80)</f>
+        <v>0.98039215686274506</v>
+      </c>
+      <c r="Q80">
+        <f>P80-P41</f>
+        <v>5.0392156862745008E-2</v>
+      </c>
+      <c r="S80" t="s">
+        <v>106</v>
+      </c>
+      <c r="T80">
+        <v>70</v>
+      </c>
+      <c r="U80">
+        <v>7</v>
+      </c>
+      <c r="V80">
+        <f>T80/(T80+U80)</f>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81">
+        <v>87</v>
+      </c>
+      <c r="C81">
+        <v>7</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ref="D81:D96" si="16">B81/(B81+C81)</f>
+        <v>0.92553191489361697</v>
+      </c>
+      <c r="E81">
+        <f t="shared" ref="E81:E96" si="17">D81-D42</f>
+        <v>-9.9519560741249125E-3</v>
+      </c>
+      <c r="G81" t="s">
+        <v>19</v>
+      </c>
+      <c r="H81">
+        <v>76</v>
+      </c>
+      <c r="I81">
+        <v>3</v>
+      </c>
+      <c r="J81">
+        <f t="shared" ref="J81:J96" si="18">H81/(H81+I81)</f>
+        <v>0.96202531645569622</v>
+      </c>
+      <c r="K81">
+        <f t="shared" ref="K81:K96" si="19">J81-J42</f>
+        <v>-2.5154170723791003E-2</v>
+      </c>
+      <c r="M81" t="s">
+        <v>72</v>
+      </c>
+      <c r="N81">
+        <v>109</v>
+      </c>
+      <c r="O81">
+        <v>6</v>
+      </c>
+      <c r="P81">
+        <f t="shared" ref="P81:P95" si="20">N81/(N81+O81)</f>
+        <v>0.94782608695652171</v>
+      </c>
+      <c r="Q81">
+        <f t="shared" ref="Q81:Q95" si="21">P81-P42</f>
+        <v>6.1861174675819974E-2</v>
+      </c>
+      <c r="S81" t="s">
+        <v>107</v>
+      </c>
+      <c r="T81">
+        <v>101</v>
+      </c>
+      <c r="U81">
+        <v>9</v>
+      </c>
+      <c r="V81">
+        <f t="shared" ref="V81:V94" si="22">T81/(T81+U81)</f>
+        <v>0.91818181818181821</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82">
+        <v>87</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="16"/>
+        <v>0.94565217391304346</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="17"/>
+        <v>2.3429951690821182E-2</v>
+      </c>
+      <c r="G82" t="s">
+        <v>20</v>
+      </c>
+      <c r="H82">
+        <v>74</v>
+      </c>
+      <c r="I82">
+        <v>3</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="18"/>
+        <v>0.96103896103896103</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="19"/>
+        <v>8.7621239519973693E-2</v>
+      </c>
+      <c r="M82" t="s">
+        <v>73</v>
+      </c>
+      <c r="N82">
+        <v>70</v>
+      </c>
+      <c r="O82">
+        <v>4</v>
+      </c>
+      <c r="P82">
+        <f t="shared" si="20"/>
+        <v>0.94594594594594594</v>
+      </c>
+      <c r="Q82">
+        <f t="shared" si="21"/>
+        <v>-4.0540540540540571E-2</v>
+      </c>
+      <c r="S82" t="s">
+        <v>108</v>
+      </c>
+      <c r="T82">
+        <v>77</v>
+      </c>
+      <c r="U82">
+        <v>13</v>
+      </c>
+      <c r="V82">
+        <f t="shared" si="22"/>
+        <v>0.85555555555555551</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83">
+        <v>91</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="16"/>
+        <v>0.978494623655914</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="17"/>
+        <v>5.1411290322580627E-2</v>
+      </c>
+      <c r="G83" t="s">
+        <v>21</v>
+      </c>
+      <c r="H83">
+        <v>92</v>
+      </c>
+      <c r="I83">
+        <v>10</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="18"/>
+        <v>0.90196078431372551</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="19"/>
+        <v>8.6426803731201263E-2</v>
+      </c>
+      <c r="M83" t="s">
+        <v>74</v>
+      </c>
+      <c r="N83">
+        <v>91</v>
+      </c>
+      <c r="O83">
+        <v>7</v>
+      </c>
+      <c r="P83">
+        <f t="shared" si="20"/>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="Q83">
+        <f t="shared" si="21"/>
+        <v>3.1664212076583209E-2</v>
+      </c>
+      <c r="S83" t="s">
+        <v>109</v>
+      </c>
+      <c r="T83">
+        <v>93</v>
+      </c>
+      <c r="U83">
+        <v>9</v>
+      </c>
+      <c r="V83">
+        <f t="shared" si="22"/>
+        <v>0.91176470588235292</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84">
+        <v>85</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="16"/>
+        <v>0.9550561797752809</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="17"/>
+        <v>1.1874361593462668E-2</v>
+      </c>
+      <c r="G84" t="s">
+        <v>22</v>
+      </c>
+      <c r="H84">
+        <v>85</v>
+      </c>
+      <c r="I84">
+        <v>8</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="18"/>
+        <v>0.91397849462365588</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="19"/>
+        <v>5.8422939068100366E-2</v>
+      </c>
+      <c r="M84" t="s">
+        <v>75</v>
+      </c>
+      <c r="N84">
+        <v>90</v>
+      </c>
+      <c r="O84">
+        <v>9</v>
+      </c>
+      <c r="P84">
+        <f t="shared" si="20"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="Q84">
+        <f t="shared" si="21"/>
+        <v>-5.93301435406699E-2</v>
+      </c>
+      <c r="S84" t="s">
+        <v>110</v>
+      </c>
+      <c r="T84">
+        <v>75</v>
+      </c>
+      <c r="U84">
+        <v>6</v>
+      </c>
+      <c r="V84">
+        <f t="shared" si="22"/>
+        <v>0.92592592592592593</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <v>7</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="16"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="17"/>
+        <v>-5.4195804195804165E-2</v>
+      </c>
+      <c r="G85" t="s">
+        <v>23</v>
+      </c>
+      <c r="H85">
+        <v>57</v>
+      </c>
+      <c r="I85">
+        <v>5</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="18"/>
+        <v>0.91935483870967738</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="19"/>
+        <v>3.2258064516129004E-2</v>
+      </c>
+      <c r="M85" t="s">
+        <v>76</v>
+      </c>
+      <c r="N85">
+        <v>80</v>
+      </c>
+      <c r="O85">
+        <v>8</v>
+      </c>
+      <c r="P85">
+        <f t="shared" si="20"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="Q85">
+        <f t="shared" si="21"/>
+        <v>3.4090909090909061E-2</v>
+      </c>
+      <c r="S85" t="s">
+        <v>111</v>
+      </c>
+      <c r="T85">
+        <v>66</v>
+      </c>
+      <c r="U85">
+        <v>8</v>
+      </c>
+      <c r="V85">
+        <f t="shared" si="22"/>
+        <v>0.89189189189189189</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86">
+        <v>102</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="16"/>
+        <v>0.96226415094339623</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="17"/>
+        <v>3.993405385601756E-2</v>
+      </c>
+      <c r="G86" t="s">
+        <v>24</v>
+      </c>
+      <c r="H86">
+        <v>123</v>
+      </c>
+      <c r="I86">
+        <v>7</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="18"/>
+        <v>0.94615384615384612</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="19"/>
+        <v>1.0153846153846069E-2</v>
+      </c>
+      <c r="M86" t="s">
+        <v>77</v>
+      </c>
+      <c r="N86">
+        <v>75</v>
+      </c>
+      <c r="O86">
+        <v>4</v>
+      </c>
+      <c r="P86">
+        <f t="shared" si="20"/>
+        <v>0.94936708860759489</v>
+      </c>
+      <c r="Q86">
+        <f t="shared" si="21"/>
+        <v>-1.1671872431366137E-2</v>
+      </c>
+      <c r="S86" t="s">
+        <v>112</v>
+      </c>
+      <c r="T86">
+        <v>90</v>
+      </c>
+      <c r="U86">
+        <v>7</v>
+      </c>
+      <c r="V86">
+        <f t="shared" si="22"/>
+        <v>0.92783505154639179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>89</v>
+      </c>
+      <c r="C87">
+        <v>9</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="16"/>
+        <v>0.90816326530612246</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="17"/>
+        <v>3.3163265306122458E-2</v>
+      </c>
+      <c r="G87" t="s">
+        <v>25</v>
+      </c>
+      <c r="H87">
+        <v>87</v>
+      </c>
+      <c r="I87">
+        <v>3</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="18"/>
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="19"/>
+        <v>6.3440860215053796E-2</v>
+      </c>
+      <c r="M87" t="s">
+        <v>78</v>
+      </c>
+      <c r="N87">
+        <v>82</v>
+      </c>
+      <c r="O87">
+        <v>4</v>
+      </c>
+      <c r="P87">
+        <f t="shared" si="20"/>
+        <v>0.95348837209302328</v>
+      </c>
+      <c r="Q87">
+        <f t="shared" si="21"/>
+        <v>3.6821705426356655E-2</v>
+      </c>
+      <c r="S87" t="s">
+        <v>113</v>
+      </c>
+      <c r="T87">
+        <v>68</v>
+      </c>
+      <c r="U87">
+        <v>8</v>
+      </c>
+      <c r="V87">
+        <f t="shared" si="22"/>
+        <v>0.89473684210526316</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88">
+        <v>69</v>
+      </c>
+      <c r="C88">
+        <v>6</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="16"/>
+        <v>0.92</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="17"/>
+        <v>2.9589041095890445E-2</v>
+      </c>
+      <c r="G88" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88">
+        <v>97</v>
+      </c>
+      <c r="I88">
+        <v>9</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="18"/>
+        <v>0.91509433962264153</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="19"/>
+        <v>2.9380053908355852E-2</v>
+      </c>
+      <c r="M88" t="s">
+        <v>79</v>
+      </c>
+      <c r="N88">
+        <v>69</v>
+      </c>
+      <c r="O88">
+        <v>13</v>
+      </c>
+      <c r="P88">
+        <f t="shared" si="20"/>
+        <v>0.84146341463414631</v>
+      </c>
+      <c r="Q88">
+        <f t="shared" si="21"/>
+        <v>-8.3536585365853733E-2</v>
+      </c>
+      <c r="S88" t="s">
+        <v>114</v>
+      </c>
+      <c r="T88">
+        <v>70</v>
+      </c>
+      <c r="U88">
+        <v>8</v>
+      </c>
+      <c r="V88">
+        <f t="shared" si="22"/>
+        <v>0.89743589743589747</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="16"/>
+        <v>0.96703296703296704</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="17"/>
+        <v>5.8986990021472785E-2</v>
+      </c>
+      <c r="G89" t="s">
+        <v>27</v>
+      </c>
+      <c r="H89">
+        <v>85</v>
+      </c>
+      <c r="I89">
+        <v>2</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="18"/>
+        <v>0.97701149425287359</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="19"/>
+        <v>8.6901604142983535E-2</v>
+      </c>
+      <c r="M89" t="s">
+        <v>80</v>
+      </c>
+      <c r="N89">
+        <v>76</v>
+      </c>
+      <c r="O89">
+        <v>5</v>
+      </c>
+      <c r="P89">
+        <f t="shared" si="20"/>
+        <v>0.93827160493827155</v>
+      </c>
+      <c r="Q89">
+        <f t="shared" si="21"/>
+        <v>1.5194681861348425E-2</v>
+      </c>
+      <c r="S89" t="s">
+        <v>115</v>
+      </c>
+      <c r="T89">
+        <v>83</v>
+      </c>
+      <c r="U89">
+        <v>4</v>
+      </c>
+      <c r="V89">
+        <f t="shared" si="22"/>
+        <v>0.95402298850574707</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90">
+        <v>69</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="16"/>
+        <v>0.93243243243243246</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="17"/>
+        <v>1.5765765765765827E-2</v>
+      </c>
+      <c r="G90" t="s">
+        <v>28</v>
+      </c>
+      <c r="H90">
+        <v>79</v>
+      </c>
+      <c r="I90">
+        <v>10</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="18"/>
+        <v>0.88764044943820219</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="19"/>
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="M90" t="s">
+        <v>81</v>
+      </c>
+      <c r="N90">
+        <v>102</v>
+      </c>
+      <c r="O90">
+        <v>3</v>
+      </c>
+      <c r="P90">
+        <f t="shared" si="20"/>
+        <v>0.97142857142857142</v>
+      </c>
+      <c r="Q90">
+        <f t="shared" si="21"/>
+        <v>2.8571428571428581E-2</v>
+      </c>
+      <c r="S90" t="s">
+        <v>116</v>
+      </c>
+      <c r="T90">
+        <v>71</v>
+      </c>
+      <c r="U90">
+        <v>19</v>
+      </c>
+      <c r="V90">
+        <f t="shared" si="22"/>
+        <v>0.78888888888888886</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91">
+        <v>81</v>
+      </c>
+      <c r="C91">
+        <v>8</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="16"/>
+        <v>0.9101123595505618</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="17"/>
+        <v>-3.1064111037673481E-2</v>
+      </c>
+      <c r="G91" t="s">
+        <v>29</v>
+      </c>
+      <c r="H91">
+        <v>91</v>
+      </c>
+      <c r="I91">
+        <v>6</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="18"/>
+        <v>0.93814432989690721</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="19"/>
+        <v>4.9255441008018375E-2</v>
+      </c>
+      <c r="M91" t="s">
+        <v>82</v>
+      </c>
+      <c r="N91">
+        <v>86</v>
+      </c>
+      <c r="O91">
+        <v>3</v>
+      </c>
+      <c r="P91">
+        <f t="shared" si="20"/>
+        <v>0.9662921348314607</v>
+      </c>
+      <c r="Q91">
+        <f t="shared" si="21"/>
+        <v>4.4069912609238426E-2</v>
+      </c>
+      <c r="S91" t="s">
+        <v>117</v>
+      </c>
+      <c r="T91">
+        <v>77</v>
+      </c>
+      <c r="U91">
+        <v>5</v>
+      </c>
+      <c r="V91">
+        <f t="shared" si="22"/>
+        <v>0.93902439024390238</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92">
+        <v>108</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="16"/>
+        <v>0.98181818181818181</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="17"/>
+        <v>5.5212677231025853E-2</v>
+      </c>
+      <c r="G92" t="s">
+        <v>30</v>
+      </c>
+      <c r="H92">
+        <v>79</v>
+      </c>
+      <c r="I92">
+        <v>13</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="18"/>
+        <v>0.85869565217391308</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="19"/>
+        <v>1.2541806020066937E-2</v>
+      </c>
+      <c r="M92" t="s">
+        <v>83</v>
+      </c>
+      <c r="N92">
+        <v>100</v>
+      </c>
+      <c r="O92">
+        <v>5</v>
+      </c>
+      <c r="P92">
+        <f t="shared" si="20"/>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="Q92">
+        <f t="shared" si="21"/>
+        <v>7.6190476190476142E-2</v>
+      </c>
+      <c r="S92" t="s">
+        <v>118</v>
+      </c>
+      <c r="T92">
+        <v>106</v>
+      </c>
+      <c r="U92">
+        <v>7</v>
+      </c>
+      <c r="V92">
+        <f t="shared" si="22"/>
+        <v>0.93805309734513276</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93">
+        <v>68</v>
+      </c>
+      <c r="C93">
+        <v>6</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="16"/>
+        <v>0.91891891891891897</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="17"/>
+        <v>2.2522522522523403E-3</v>
+      </c>
+      <c r="G93" t="s">
+        <v>31</v>
+      </c>
+      <c r="H93">
+        <v>90</v>
+      </c>
+      <c r="I93">
+        <v>5</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="18"/>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="K93">
+        <f t="shared" si="19"/>
+        <v>8.736842105263154E-2</v>
+      </c>
+      <c r="M93" t="s">
+        <v>84</v>
+      </c>
+      <c r="N93">
+        <v>97</v>
+      </c>
+      <c r="O93">
+        <v>6</v>
+      </c>
+      <c r="P93">
+        <f t="shared" si="20"/>
+        <v>0.94174757281553401</v>
+      </c>
+      <c r="Q93">
+        <f t="shared" si="21"/>
+        <v>-1.8252427184465958E-2</v>
+      </c>
+      <c r="S93" t="s">
+        <v>119</v>
+      </c>
+      <c r="T93">
+        <v>104</v>
+      </c>
+      <c r="U93">
+        <v>11</v>
+      </c>
+      <c r="V93">
+        <f t="shared" si="22"/>
+        <v>0.90434782608695652</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94">
+        <v>87</v>
+      </c>
+      <c r="C94">
+        <v>15</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="16"/>
+        <v>0.8529411764705882</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="17"/>
+        <v>-1.1642156862745168E-2</v>
+      </c>
+      <c r="G94" t="s">
+        <v>32</v>
+      </c>
+      <c r="H94">
+        <v>68</v>
+      </c>
+      <c r="I94">
+        <v>8</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="18"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="19"/>
+        <v>-1.3157894736842146E-2</v>
+      </c>
+      <c r="M94" t="s">
+        <v>85</v>
+      </c>
+      <c r="N94">
+        <v>87</v>
+      </c>
+      <c r="O94">
+        <v>7</v>
+      </c>
+      <c r="P94">
+        <f t="shared" si="20"/>
+        <v>0.92553191489361697</v>
+      </c>
+      <c r="Q94">
+        <f t="shared" si="21"/>
+        <v>3.0795072788353806E-2</v>
+      </c>
+      <c r="S94" t="s">
+        <v>120</v>
+      </c>
+      <c r="T94">
+        <f>SUM(T80:T93)</f>
+        <v>1151</v>
+      </c>
+      <c r="U94">
+        <f>SUM(U80:U93)</f>
+        <v>121</v>
+      </c>
+      <c r="V94">
+        <f t="shared" si="22"/>
+        <v>0.90487421383647804</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>11</v>
+      </c>
+      <c r="B95">
+        <v>91</v>
+      </c>
+      <c r="C95">
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="16"/>
+        <v>0.90099009900990101</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="17"/>
+        <v>6.2532569046378494E-3</v>
+      </c>
+      <c r="G95" t="s">
+        <v>33</v>
+      </c>
+      <c r="H95">
+        <v>82</v>
+      </c>
+      <c r="I95">
+        <v>9</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="18"/>
+        <v>0.90109890109890112</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="19"/>
+        <v>3.5930361773058417E-2</v>
+      </c>
+      <c r="M95" t="s">
+        <v>87</v>
+      </c>
+      <c r="N95">
+        <f>SUM(N80:N94)</f>
+        <v>1314</v>
+      </c>
+      <c r="O95">
+        <f>SUM(O80:O94)</f>
+        <v>86</v>
+      </c>
+      <c r="P95">
+        <f t="shared" si="20"/>
+        <v>0.93857142857142861</v>
+      </c>
+      <c r="Q95">
+        <f t="shared" si="21"/>
+        <v>1.5995451726276699E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96">
+        <f>SUM(B80:B95)</f>
+        <v>1394</v>
+      </c>
+      <c r="C96">
+        <f>SUM(C80:C95)</f>
+        <v>98</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="16"/>
+        <v>0.93431635388739942</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="17"/>
+        <v>2.1421978030060629E-2</v>
+      </c>
+      <c r="G96" t="s">
+        <v>34</v>
+      </c>
+      <c r="H96">
+        <f>SUM(H80:H95)</f>
+        <v>1355</v>
+      </c>
+      <c r="I96">
+        <f>SUM(I80:I95)</f>
+        <v>107</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="18"/>
+        <v>0.926812585499316</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="19"/>
+        <v>4.0883623750682108E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N98" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O98" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q98" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99">
+        <v>114</v>
+      </c>
+      <c r="C99">
+        <v>13</v>
+      </c>
+      <c r="D99">
+        <f>B99/(B99+C99)</f>
+        <v>0.89763779527559051</v>
+      </c>
+      <c r="E99">
+        <f>D99-D60</f>
+        <v>4.4924616981016907E-2</v>
+      </c>
+      <c r="G99" t="s">
+        <v>54</v>
+      </c>
+      <c r="H99">
+        <v>84</v>
+      </c>
+      <c r="I99">
+        <v>13</v>
+      </c>
+      <c r="J99">
+        <f>H99/(H99+I99)</f>
+        <v>0.865979381443299</v>
+      </c>
+      <c r="K99">
+        <f>J99-J60</f>
+        <v>-1.0309278350515427E-2</v>
+      </c>
+      <c r="M99" t="s">
+        <v>89</v>
+      </c>
+      <c r="N99">
+        <v>94</v>
+      </c>
+      <c r="O99">
+        <v>4</v>
+      </c>
+      <c r="P99">
+        <f>N99/(N99+O99)</f>
+        <v>0.95918367346938771</v>
+      </c>
+      <c r="Q99">
+        <f>P99-P60</f>
+        <v>8.7896544756516426E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>69</v>
+      </c>
+      <c r="B100">
+        <v>87</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <f t="shared" ref="D100:D115" si="23">B100/(B100+C100)</f>
+        <v>0.95604395604395609</v>
+      </c>
+      <c r="E100">
+        <f t="shared" ref="E100:E115" si="24">D100-D61</f>
+        <v>1.0989010989011061E-2</v>
+      </c>
+      <c r="G100" t="s">
+        <v>55</v>
+      </c>
+      <c r="H100">
+        <v>76</v>
+      </c>
+      <c r="I100">
+        <v>6</v>
+      </c>
+      <c r="J100">
+        <f t="shared" ref="J100:J109" si="25">H100/(H100+I100)</f>
+        <v>0.92682926829268297</v>
+      </c>
+      <c r="K100">
+        <f t="shared" ref="K100:K114" si="26">J100-J61</f>
+        <v>1.4329268292682995E-2</v>
+      </c>
+      <c r="M100" t="s">
+        <v>90</v>
+      </c>
+      <c r="N100">
+        <v>79</v>
+      </c>
+      <c r="O100">
+        <v>4</v>
+      </c>
+      <c r="P100">
+        <f t="shared" ref="P100:P114" si="27">N100/(N100+O100)</f>
+        <v>0.95180722891566261</v>
+      </c>
+      <c r="Q100">
+        <f t="shared" ref="Q100:Q114" si="28">P100-P61</f>
+        <v>3.7173082574199157E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>39</v>
+      </c>
+      <c r="B101">
+        <v>95</v>
+      </c>
+      <c r="C101">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="23"/>
+        <v>0.95959595959595956</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="24"/>
+        <v>-1.0101010101010166E-2</v>
+      </c>
+      <c r="G101" t="s">
+        <v>56</v>
+      </c>
+      <c r="H101">
+        <v>93</v>
+      </c>
+      <c r="I101">
+        <v>9</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="25"/>
+        <v>0.91176470588235292</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="26"/>
+        <v>3.0576587070471728E-2</v>
+      </c>
+      <c r="M101" t="s">
+        <v>91</v>
+      </c>
+      <c r="N101">
+        <v>76</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="P101">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q101">
+        <f t="shared" si="28"/>
+        <v>1.2987012987012991E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>40</v>
+      </c>
+      <c r="B102">
+        <v>80</v>
+      </c>
+      <c r="C102">
+        <v>6</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="23"/>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="24"/>
+        <v>7.1409028727770218E-2</v>
+      </c>
+      <c r="G102" t="s">
+        <v>57</v>
+      </c>
+      <c r="H102">
+        <v>64</v>
+      </c>
+      <c r="I102">
+        <v>10</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="25"/>
+        <v>0.86486486486486491</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="26"/>
+        <v>-3.5561877667140696E-3</v>
+      </c>
+      <c r="M102" t="s">
+        <v>92</v>
+      </c>
+      <c r="N102">
+        <v>86</v>
+      </c>
+      <c r="O102">
+        <v>5</v>
+      </c>
+      <c r="P102">
+        <f t="shared" si="27"/>
+        <v>0.94505494505494503</v>
+      </c>
+      <c r="Q102">
+        <f t="shared" si="28"/>
+        <v>4.2881032011466758E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>41</v>
+      </c>
+      <c r="B103">
+        <v>83</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="23"/>
+        <v>0.89247311827956988</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="24"/>
+        <v>8.1946802490096227E-2</v>
+      </c>
+      <c r="G103" t="s">
+        <v>58</v>
+      </c>
+      <c r="H103">
+        <v>71</v>
+      </c>
+      <c r="I103">
+        <v>7</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="25"/>
+        <v>0.91025641025641024</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="26"/>
+        <v>-1.5669515669515688E-2</v>
+      </c>
+      <c r="M103" t="s">
+        <v>93</v>
+      </c>
+      <c r="N103">
+        <v>87</v>
+      </c>
+      <c r="O103">
+        <v>4</v>
+      </c>
+      <c r="P103">
+        <f t="shared" si="27"/>
+        <v>0.95604395604395609</v>
+      </c>
+      <c r="Q103">
+        <f t="shared" si="28"/>
+        <v>4.206546142030021E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>43</v>
+      </c>
+      <c r="B104">
+        <v>88</v>
+      </c>
+      <c r="C104">
+        <v>15</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="23"/>
+        <v>0.85436893203883491</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="24"/>
+        <v>-3.5631067961165108E-2</v>
+      </c>
+      <c r="G104" t="s">
+        <v>59</v>
+      </c>
+      <c r="H104">
+        <v>87</v>
+      </c>
+      <c r="I104">
+        <v>5</v>
+      </c>
+      <c r="J104">
+        <f t="shared" si="25"/>
+        <v>0.94565217391304346</v>
+      </c>
+      <c r="K104">
+        <f t="shared" si="26"/>
+        <v>1.2318840579710111E-2</v>
+      </c>
+      <c r="M104" t="s">
+        <v>94</v>
+      </c>
+      <c r="N104">
+        <v>88</v>
+      </c>
+      <c r="O104">
+        <v>6</v>
+      </c>
+      <c r="P104">
+        <f t="shared" si="27"/>
+        <v>0.93617021276595747</v>
+      </c>
+      <c r="Q104">
+        <f t="shared" si="28"/>
+        <v>5.8619192357794225E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>42</v>
+      </c>
+      <c r="B105">
+        <v>93</v>
+      </c>
+      <c r="C105">
+        <v>9</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="23"/>
+        <v>0.91176470588235292</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="24"/>
+        <v>6.7104511707595682E-2</v>
+      </c>
+      <c r="G105" t="s">
+        <v>60</v>
+      </c>
+      <c r="H105">
+        <v>109</v>
+      </c>
+      <c r="I105">
+        <v>1</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="25"/>
+        <v>0.99090909090909096</v>
+      </c>
+      <c r="K105">
+        <f t="shared" si="26"/>
+        <v>3.6780650542118432E-2</v>
+      </c>
+      <c r="M105" t="s">
+        <v>95</v>
+      </c>
+      <c r="N105">
+        <v>86</v>
+      </c>
+      <c r="O105">
+        <v>3</v>
+      </c>
+      <c r="P105">
+        <f t="shared" si="27"/>
+        <v>0.9662921348314607</v>
+      </c>
+      <c r="Q105">
+        <f t="shared" si="28"/>
+        <v>6.4118221787982432E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106">
+        <v>103</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="23"/>
+        <v>0.97169811320754718</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="24"/>
+        <v>3.7735849056603765E-2</v>
+      </c>
+      <c r="G106" t="s">
+        <v>61</v>
+      </c>
+      <c r="H106">
+        <v>84</v>
+      </c>
+      <c r="I106">
+        <v>4</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="25"/>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="K106">
+        <f t="shared" si="26"/>
+        <v>4.7568710359408128E-2</v>
+      </c>
+      <c r="M106" t="s">
+        <v>96</v>
+      </c>
+      <c r="N106">
+        <v>121</v>
+      </c>
+      <c r="O106">
+        <v>7</v>
+      </c>
+      <c r="P106">
+        <f t="shared" si="27"/>
+        <v>0.9453125</v>
+      </c>
+      <c r="Q106">
+        <f t="shared" si="28"/>
+        <v>4.7674704724409489E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>45</v>
+      </c>
+      <c r="B107">
+        <v>109</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="23"/>
+        <v>0.99090909090909096</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="24"/>
+        <v>4.6464646464646542E-2</v>
+      </c>
+      <c r="G107" t="s">
+        <v>62</v>
+      </c>
+      <c r="H107">
+        <v>78</v>
+      </c>
+      <c r="I107">
+        <v>3</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="25"/>
+        <v>0.96296296296296291</v>
+      </c>
+      <c r="K107">
+        <f t="shared" si="26"/>
+        <v>7.6887013595874354E-2</v>
+      </c>
+      <c r="M107" t="s">
+        <v>97</v>
+      </c>
+      <c r="N107">
+        <v>77</v>
+      </c>
+      <c r="O107">
+        <v>3</v>
+      </c>
+      <c r="P107">
+        <f t="shared" si="27"/>
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="Q107">
+        <f t="shared" si="28"/>
+        <v>9.6646341463414664E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>46</v>
+      </c>
+      <c r="B108">
+        <v>78</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="23"/>
+        <v>0.96296296296296291</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="24"/>
+        <v>6.8845315904139337E-2</v>
+      </c>
+      <c r="G108" t="s">
+        <v>63</v>
+      </c>
+      <c r="H108">
+        <v>86</v>
+      </c>
+      <c r="I108">
+        <v>4</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="25"/>
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="K108">
+        <f t="shared" si="26"/>
+        <v>1.237373737373737E-2</v>
+      </c>
+      <c r="M108" t="s">
+        <v>98</v>
+      </c>
+      <c r="N108">
+        <v>79</v>
+      </c>
+      <c r="O108">
+        <v>6</v>
+      </c>
+      <c r="P108">
+        <f t="shared" si="27"/>
+        <v>0.92941176470588238</v>
+      </c>
+      <c r="Q108">
+        <f t="shared" si="28"/>
+        <v>3.406292749658002E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>47</v>
+      </c>
+      <c r="B109">
+        <v>78</v>
+      </c>
+      <c r="C109">
+        <v>15</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="23"/>
+        <v>0.83870967741935487</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="24"/>
+        <v>-6.8267066766691586E-2</v>
+      </c>
+      <c r="G109" t="s">
+        <v>64</v>
+      </c>
+      <c r="H109">
+        <v>105</v>
+      </c>
+      <c r="I109">
+        <v>4</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="25"/>
+        <v>0.96330275229357798</v>
+      </c>
+      <c r="K109">
+        <f t="shared" si="26"/>
+        <v>1.7848206839032543E-2</v>
+      </c>
+      <c r="M109" t="s">
+        <v>99</v>
+      </c>
+      <c r="N109">
+        <v>94</v>
+      </c>
+      <c r="O109">
+        <v>9</v>
+      </c>
+      <c r="P109">
+        <f t="shared" si="27"/>
+        <v>0.91262135922330101</v>
+      </c>
+      <c r="Q109">
+        <f t="shared" si="28"/>
+        <v>5.9680182752712807E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>48</v>
+      </c>
+      <c r="B110">
+        <v>75</v>
+      </c>
+      <c r="C110">
+        <v>12</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="23"/>
+        <v>0.86206896551724133</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="24"/>
+        <v>1.1494252873563204E-2</v>
+      </c>
+      <c r="G110" t="s">
+        <v>70</v>
+      </c>
+      <c r="H110">
+        <v>74</v>
+      </c>
+      <c r="I110">
+        <v>3</v>
+      </c>
+      <c r="J110">
+        <f>H110/(H110+I110)</f>
+        <v>0.96103896103896103</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="26"/>
+        <v>1.5795015795015965E-3</v>
+      </c>
+      <c r="M110" t="s">
+        <v>100</v>
+      </c>
+      <c r="N110">
+        <v>87</v>
+      </c>
+      <c r="O110">
+        <v>10</v>
+      </c>
+      <c r="P110">
+        <f t="shared" si="27"/>
+        <v>0.89690721649484539</v>
+      </c>
+      <c r="Q110">
+        <f t="shared" si="28"/>
+        <v>2.3223005968529553E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>49</v>
+      </c>
+      <c r="B111">
+        <v>89</v>
+      </c>
+      <c r="C111">
+        <v>7</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="23"/>
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="24"/>
+        <v>2.5984432234432253E-2</v>
+      </c>
+      <c r="G111" t="s">
+        <v>65</v>
+      </c>
+      <c r="H111">
+        <v>76</v>
+      </c>
+      <c r="I111">
+        <v>6</v>
+      </c>
+      <c r="J111">
+        <f>H111/(H111+I111)</f>
+        <v>0.92682926829268297</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="26"/>
+        <v>-8.8157508081099234E-4</v>
+      </c>
+      <c r="M111" t="s">
+        <v>104</v>
+      </c>
+      <c r="N111">
+        <v>81</v>
+      </c>
+      <c r="O111">
+        <v>5</v>
+      </c>
+      <c r="P111">
+        <f t="shared" si="27"/>
+        <v>0.94186046511627908</v>
+      </c>
+      <c r="Q111">
+        <f t="shared" si="28"/>
+        <v>0.15534361118369477</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>50</v>
+      </c>
+      <c r="B112">
+        <v>96</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="23"/>
+        <v>0.98969072164948457</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="24"/>
+        <v>6.9690721649484533E-2</v>
+      </c>
+      <c r="G112" t="s">
+        <v>66</v>
+      </c>
+      <c r="H112">
+        <v>73</v>
+      </c>
+      <c r="I112">
+        <v>4</v>
+      </c>
+      <c r="J112">
+        <f>H112/(H112+I112)</f>
+        <v>0.94805194805194803</v>
+      </c>
+      <c r="K112">
+        <f t="shared" si="26"/>
+        <v>4.2646542646542662E-2</v>
+      </c>
+      <c r="M112" t="s">
+        <v>103</v>
+      </c>
+      <c r="N112">
+        <v>100</v>
+      </c>
+      <c r="O112">
+        <v>4</v>
+      </c>
+      <c r="P112">
+        <f t="shared" si="27"/>
+        <v>0.96153846153846156</v>
+      </c>
+      <c r="Q112">
+        <f t="shared" si="28"/>
+        <v>0.10015232292460019</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>51</v>
+      </c>
+      <c r="B113">
+        <v>70</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="23"/>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="24"/>
+        <v>6.6816816816816837E-2</v>
+      </c>
+      <c r="G113" t="s">
+        <v>67</v>
+      </c>
+      <c r="H113">
+        <v>75</v>
+      </c>
+      <c r="I113">
+        <v>7</v>
+      </c>
+      <c r="J113">
+        <f>H113/(H113+I113)</f>
+        <v>0.91463414634146345</v>
+      </c>
+      <c r="K113">
+        <f t="shared" si="26"/>
+        <v>8.1300813008130079E-2</v>
+      </c>
+      <c r="M113" t="s">
+        <v>101</v>
+      </c>
+      <c r="N113">
+        <v>79</v>
+      </c>
+      <c r="O113">
+        <v>5</v>
+      </c>
+      <c r="P113">
+        <f t="shared" si="27"/>
+        <v>0.94047619047619047</v>
+      </c>
+      <c r="Q113">
+        <f t="shared" si="28"/>
+        <v>6.0958118187033894E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>52</v>
+      </c>
+      <c r="B114">
+        <v>95</v>
+      </c>
+      <c r="C114">
+        <v>14</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="23"/>
+        <v>0.87155963302752293</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="24"/>
+        <v>2.1092343307896777E-2</v>
+      </c>
+      <c r="G114" t="s">
+        <v>68</v>
+      </c>
+      <c r="H114">
+        <f>SUM(H99:H113)</f>
+        <v>1235</v>
+      </c>
+      <c r="I114">
+        <f>SUM(I99:I113)</f>
+        <v>86</v>
+      </c>
+      <c r="J114">
+        <f>H114/(H114+I114)</f>
+        <v>0.9348978046934141</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="26"/>
+        <v>2.3312438839755534E-2</v>
+      </c>
+      <c r="M114" t="s">
+        <v>105</v>
+      </c>
+      <c r="N114">
+        <f>SUM(N99:N113)</f>
+        <v>1314</v>
+      </c>
+      <c r="O114">
+        <f>SUM(O99:O113)</f>
+        <v>75</v>
+      </c>
+      <c r="P114">
+        <f t="shared" si="27"/>
+        <v>0.94600431965442766</v>
+      </c>
+      <c r="Q114">
+        <f t="shared" si="28"/>
+        <v>6.1718605368713431E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>53</v>
+      </c>
+      <c r="B115">
+        <f>SUM(B99:B114)</f>
+        <v>1433</v>
+      </c>
+      <c r="C115">
+        <f>SUM(C99:C114)</f>
+        <v>119</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="23"/>
+        <v>0.92332474226804129</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="24"/>
+        <v>3.1345440845014116E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>